<commit_message>
Updated plots and excel sheets
</commit_message>
<xml_diff>
--- a/lfd_package/results/miami_fl/miami_fl_results.xlsx
+++ b/lfd_package/results/miami_fl/miami_fl_results.xlsx
@@ -478,7 +478,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>440.19</v>
+        <v>413.13</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -491,7 +491,7 @@
         </is>
       </c>
       <c r="L2" t="n">
-        <v>-1096795.83</v>
+        <v>-989969.67</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
@@ -499,7 +499,7 @@
         </is>
       </c>
       <c r="N2" t="n">
-        <v>-19770.53</v>
+        <v>-19726.16</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="P2" t="n">
-        <v>-1057891.51</v>
+        <v>-1061202</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
@@ -515,7 +515,7 @@
         </is>
       </c>
       <c r="R2" t="n">
-        <v>-3538703.21</v>
+        <v>-3083621.63</v>
       </c>
       <c r="S2" t="inlineStr">
         <is>
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>112.85</v>
+        <v>98.47</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -543,7 +543,7 @@
         </is>
       </c>
       <c r="L3" t="n">
-        <v>317295.05</v>
+        <v>287017.77</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -551,7 +551,7 @@
         </is>
       </c>
       <c r="N3" t="n">
-        <v>15244.17</v>
+        <v>15209.64</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -559,7 +559,7 @@
         </is>
       </c>
       <c r="P3" t="n">
-        <v>284611.75</v>
+        <v>284915.98</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="R3" t="n">
-        <v>440189.6</v>
+        <v>413128.48</v>
       </c>
       <c r="S3" t="inlineStr">
         <is>
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>45.917</v>
+        <v>43.269</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -595,7 +595,7 @@
         </is>
       </c>
       <c r="L4" t="n">
-        <v>-779500.78</v>
+        <v>-702951.9</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
@@ -603,7 +603,7 @@
         </is>
       </c>
       <c r="N4" t="n">
-        <v>-4526.37</v>
+        <v>-4516.53</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -611,7 +611,7 @@
         </is>
       </c>
       <c r="P4" t="n">
-        <v>-773279.76</v>
+        <v>-776286.02</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
@@ -619,7 +619,7 @@
         </is>
       </c>
       <c r="R4" t="n">
-        <v>-3098513.61</v>
+        <v>-2670493.16</v>
       </c>
       <c r="S4" t="inlineStr">
         <is>
@@ -634,7 +634,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>90.652</v>
+        <v>65.117</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -685,7 +685,7 @@
         </is>
       </c>
       <c r="L7" t="n">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="M7" t="inlineStr">
         <is>
@@ -700,7 +700,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>40.59</v>
+        <v>35.34</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -708,7 +708,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>152.976</v>
+        <v>17.303</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -716,7 +716,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>90.65000000000001</v>
+        <v>65.12</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -729,7 +729,7 @@
         </is>
       </c>
       <c r="L8" t="n">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
@@ -760,7 +760,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>90.65000000000001</v>
+        <v>65.12</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -773,7 +773,7 @@
         </is>
       </c>
       <c r="L9" t="n">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
@@ -796,7 +796,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>64.096</v>
+        <v>0</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -804,7 +804,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>90.65000000000001</v>
+        <v>65.12</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -817,7 +817,7 @@
         </is>
       </c>
       <c r="L10" t="n">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>112.85</v>
+        <v>98.47</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -848,7 +848,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>90.65000000000001</v>
+        <v>65.12</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -861,7 +861,7 @@
         </is>
       </c>
       <c r="L11" t="n">
-        <v>177</v>
+        <v>154</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>
@@ -929,7 +929,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>317295.05</v>
+        <v>287017.77</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -937,7 +937,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>15244.17</v>
+        <v>15209.64</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -945,7 +945,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>284611.75</v>
+        <v>284915.98</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -953,7 +953,7 @@
         </is>
       </c>
       <c r="H14" t="n">
-        <v>440189.6</v>
+        <v>413128.48</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
@@ -966,16 +966,16 @@
         </is>
       </c>
       <c r="L14" t="n">
-        <v>1214.46</v>
+        <v>1146.33</v>
       </c>
       <c r="M14" t="n">
-        <v>415.83</v>
+        <v>423.93</v>
       </c>
       <c r="N14" t="n">
-        <v>1176.09</v>
+        <v>1108.05</v>
       </c>
       <c r="O14" t="n">
-        <v>498.1</v>
+        <v>429.22</v>
       </c>
       <c r="P14" t="n">
         <v>0</v>
@@ -988,7 +988,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>122894.55</v>
+        <v>126110.71</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -996,7 +996,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>424945.44</v>
+        <v>397918.84</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -1004,7 +1004,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>155577.85</v>
+        <v>128212.5</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1025,19 +1025,19 @@
         </is>
       </c>
       <c r="L15" t="n">
-        <v>8021.23</v>
+        <v>7944.79</v>
       </c>
       <c r="M15" t="n">
-        <v>33345.08</v>
+        <v>30802.14</v>
       </c>
       <c r="N15" t="n">
-        <v>8477.709999999999</v>
+        <v>8400.25</v>
       </c>
       <c r="O15" t="n">
         <v>32446.82</v>
       </c>
       <c r="P15" t="n">
-        <v>89726.12</v>
+        <v>79142.33</v>
       </c>
     </row>
     <row r="16">
@@ -1055,7 +1055,7 @@
       </c>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="n">
-        <v>21988.25</v>
+        <v>21684.02</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1063,7 +1063,7 @@
         </is>
       </c>
       <c r="H16" t="n">
-        <v>548401.74</v>
+        <v>449447.89</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
@@ -1081,7 +1081,7 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>140184.11</v>
+        <v>122049.98</v>
       </c>
       <c r="N16" t="n">
         <v>7222.1</v>
@@ -1090,7 +1090,7 @@
         <v>120866.9</v>
       </c>
       <c r="P16" t="n">
-        <v>389719.41</v>
+        <v>340042.18</v>
       </c>
     </row>
     <row r="17">
@@ -1100,7 +1100,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>594008.0600000001</v>
+        <v>537325.96</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -1108,7 +1108,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>29383.51</v>
+        <v>29316.95</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1124,7 +1124,7 @@
         </is>
       </c>
       <c r="H17" t="n">
-        <v>1850741.85</v>
+        <v>1614829.22</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
@@ -1142,16 +1142,16 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>9518.85</v>
+        <v>8610.530000000001</v>
       </c>
       <c r="N17" t="n">
-        <v>457.32</v>
+        <v>456.29</v>
       </c>
       <c r="O17" t="n">
         <v>9198</v>
       </c>
       <c r="P17" t="n">
-        <v>29657.74</v>
+        <v>25877.29</v>
       </c>
     </row>
     <row r="18">
@@ -1161,7 +1161,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>223.62</v>
+        <v>17.3</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -1169,7 +1169,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>2652.33</v>
+        <v>2686.09</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1177,7 +1177,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>72.45999999999999</v>
+        <v>0</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1203,13 +1203,13 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>3206.38</v>
+        <v>362.68</v>
       </c>
       <c r="N18" t="n">
         <v>463.58</v>
       </c>
       <c r="O18" t="n">
-        <v>1343.44</v>
+        <v>0</v>
       </c>
       <c r="P18" t="n">
         <v>0</v>
@@ -1230,7 +1230,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>17372</v>
+        <v>14788.6</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -1294,10 +1294,10 @@
         <v>0</v>
       </c>
       <c r="O20" t="n">
-        <v>5079.04</v>
+        <v>5057.65</v>
       </c>
       <c r="P20" t="n">
-        <v>47574.38</v>
+        <v>39604.92</v>
       </c>
     </row>
     <row r="21">
@@ -1337,16 +1337,16 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-4.21</v>
+        <v>-3.98</v>
       </c>
       <c r="N21" t="n">
-        <v>-8.779999999999999</v>
+        <v>-8.800000000000001</v>
       </c>
       <c r="O21" t="n">
-        <v>-4.39</v>
+        <v>-4.33</v>
       </c>
       <c r="P21" t="n">
-        <v>-6.23</v>
+        <v>-6.04</v>
       </c>
     </row>
     <row r="22">
@@ -1356,7 +1356,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>72.08</v>
+        <v>69.47</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1364,7 +1364,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>3.46</v>
+        <v>3.68</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1372,7 +1372,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>64.66</v>
+        <v>68.97</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1398,16 +1398,16 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-2.63</v>
+        <v>-2.49</v>
       </c>
       <c r="N22" t="n">
-        <v>-5.49</v>
+        <v>-5.5</v>
       </c>
       <c r="O22" t="n">
-        <v>-2.74</v>
+        <v>-2.71</v>
       </c>
       <c r="P22" t="n">
-        <v>-3.89</v>
+        <v>-3.77</v>
       </c>
     </row>
     <row r="23">
@@ -1417,7 +1417,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>27.92</v>
+        <v>30.53</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1425,7 +1425,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>96.54000000000001</v>
+        <v>96.31999999999999</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1433,7 +1433,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>35.34</v>
+        <v>31.03</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1456,7 +1456,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1293.65</v>
+        <v>1241.83</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1464,7 +1464,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>63.99</v>
+        <v>67.76000000000001</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1472,7 +1472,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>1250.04</v>
+        <v>1326.55</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1480,7 +1480,7 @@
         </is>
       </c>
       <c r="H24" t="n">
-        <v>4030.6</v>
+        <v>3732.08</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
@@ -1495,7 +1495,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.49</v>
+        <v>0.04</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1503,7 +1503,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>5.78</v>
+        <v>6.21</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1511,7 +1511,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1542,7 +1542,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>37.83</v>
+        <v>34.18</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>

</xml_diff>